<commit_message>
2025 entries and wildcard update
</commit_message>
<xml_diff>
--- a/2025_results.xlsx
+++ b/2025_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nbr37_newcastle_ac_uk/Documents/MEP and Teaching/MMM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{122CAC6E-EEDB-4DCF-AB33-B654553535D0}"/>
+  <xr:revisionPtr revIDLastSave="809" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42DF1722-1B3A-42AD-92CA-51CE1933DF89}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="1770" yWindow="1215" windowWidth="26730" windowHeight="12345" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
   <si>
     <t>Round_1</t>
   </si>
@@ -638,7 +638,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P34" sqref="P34"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -936,7 +936,9 @@
       <c r="C17">
         <v>14</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="I17" s="3"/>
       <c r="K17" s="3"/>
       <c r="P17" s="3" t="s">
@@ -958,7 +960,9 @@
       <c r="A19" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C19">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
round1 the only ones results
</commit_message>
<xml_diff>
--- a/2025_results.xlsx
+++ b/2025_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="809" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42DF1722-1B3A-42AD-92CA-51CE1933DF89}"/>
+  <xr:revisionPtr revIDLastSave="817" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB2A1B18-BEDD-49FE-A13A-C36B886DE620}"/>
   <bookViews>
-    <workbookView xWindow="1770" yWindow="1215" windowWidth="26730" windowHeight="12345" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="1365" yWindow="1590" windowWidth="26730" windowHeight="12345" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
   <si>
     <t>Round_1</t>
   </si>
@@ -336,6 +336,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -637,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -969,7 +973,9 @@
       <c r="D19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E19" s="3"/>
+      <c r="E19" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="J19" s="3"/>
       <c r="O19" s="3"/>
       <c r="P19" s="3" t="s">
@@ -1005,7 +1011,9 @@
       <c r="D21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="3"/>
+      <c r="E21" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="O21" s="3"/>
       <c r="P21" s="3" t="s">
         <v>63</v>
@@ -1037,7 +1045,9 @@
       <c r="D23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E23" s="3"/>
+      <c r="E23" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3" t="s">
         <v>65</v>
@@ -1069,7 +1079,9 @@
       <c r="D25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="O25" s="3"/>
       <c r="P25" s="3" t="s">
         <v>67</v>
@@ -1101,7 +1113,9 @@
       <c r="D27" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E27" s="3"/>
+      <c r="E27" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="O27" s="3"/>
       <c r="P27" s="3" t="s">
         <v>69</v>
@@ -1133,7 +1147,9 @@
       <c r="D29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="3"/>
+      <c r="E29" s="3" t="s">
+        <v>39</v>
+      </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3" t="s">
         <v>71</v>
@@ -1166,7 +1182,9 @@
       <c r="D31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E31" s="3"/>
+      <c r="E31" s="3" t="s">
+        <v>41</v>
+      </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3" t="s">
         <v>73</v>
@@ -1198,7 +1216,9 @@
       <c r="D33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E33" s="3"/>
+      <c r="E33" s="3" t="s">
+        <v>43</v>
+      </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
         <v>75</v>

</xml_diff>

<commit_message>
round 1 roots and relics results
</commit_message>
<xml_diff>
--- a/2025_results.xlsx
+++ b/2025_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="817" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB2A1B18-BEDD-49FE-A13A-C36B886DE620}"/>
+  <xr:revisionPtr revIDLastSave="828" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36334FD6-D380-498E-B906-F4608F0A1A5A}"/>
   <bookViews>
-    <workbookView xWindow="1365" yWindow="1590" windowWidth="26730" windowHeight="12345" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="4395" yWindow="1335" windowWidth="26730" windowHeight="12345" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="80">
   <si>
     <t>Round_1</t>
   </si>
@@ -265,6 +265,15 @@
   </si>
   <si>
     <t>Fern</t>
+  </si>
+  <si>
+    <t>GinkoRhizo</t>
+  </si>
+  <si>
+    <t>Ceolacanth</t>
+  </si>
+  <si>
+    <t>Saimaa Ringed Seal</t>
   </si>
 </sst>
 </file>
@@ -642,7 +651,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -977,7 +986,9 @@
         <v>29</v>
       </c>
       <c r="J19" s="3"/>
-      <c r="O19" s="3"/>
+      <c r="O19" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="P19" s="3" t="s">
         <v>61</v>
       </c>
@@ -1014,7 +1025,9 @@
       <c r="E21" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O21" s="3"/>
+      <c r="O21" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="P21" s="3" t="s">
         <v>63</v>
       </c>
@@ -1048,7 +1061,9 @@
       <c r="E23" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="O23" s="3"/>
+      <c r="O23" s="3" t="s">
+        <v>79</v>
+      </c>
       <c r="P23" s="3" t="s">
         <v>65</v>
       </c>
@@ -1082,7 +1097,9 @@
       <c r="E25" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="3"/>
+      <c r="O25" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="P25" s="3" t="s">
         <v>67</v>
       </c>
@@ -1116,7 +1133,9 @@
       <c r="E27" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O27" s="3"/>
+      <c r="O27" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="P27" s="3" t="s">
         <v>69</v>
       </c>
@@ -1150,7 +1169,9 @@
       <c r="E29" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O29" s="3"/>
+      <c r="O29" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="P29" s="3" t="s">
         <v>71</v>
       </c>
@@ -1185,7 +1206,9 @@
       <c r="E31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="O31" s="3"/>
+      <c r="O31" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="P31" s="3" t="s">
         <v>73</v>
       </c>
@@ -1219,7 +1242,9 @@
       <c r="E33" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="O33" s="3"/>
+      <c r="O33" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="P33" s="3" t="s">
         <v>75</v>
       </c>

</xml_diff>

<commit_message>
Same and different r1 results and fixed two brackets
</commit_message>
<xml_diff>
--- a/2025_results.xlsx
+++ b/2025_results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/njw179_newcastle_ac_uk/Documents/MMM/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nbr37_newcastle_ac_uk/Documents/MEP and Teaching/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="830" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E9AC8B8-68DE-4B98-9BE3-6F85A960E74D}"/>
+  <xr:revisionPtr revIDLastSave="838" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2D76453-7F4A-4836-8812-0ABEDB806078}"/>
   <bookViews>
-    <workbookView xWindow="-25560" yWindow="1440" windowWidth="26730" windowHeight="12345" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
   <si>
     <t>Round_1</t>
   </si>
@@ -348,10 +348,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -653,8 +649,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA7A126-1676-F548-AFF2-D58DA2E40C88}">
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -710,7 +706,9 @@
       <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
       <c r="O2" s="3"/>
       <c r="P2" s="3" t="s">
         <v>45</v>
@@ -745,7 +743,9 @@
       <c r="D4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="O4" s="3"/>
       <c r="P4" s="3" t="s">
         <v>47</v>
@@ -777,7 +777,9 @@
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
       <c r="O6" s="3"/>
       <c r="P6" s="3" t="s">
         <v>49</v>
@@ -809,7 +811,9 @@
       <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3" t="s">
@@ -842,7 +846,9 @@
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
         <v>53</v>
@@ -874,7 +880,9 @@
       <c r="D12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
         <v>55</v>
@@ -907,7 +915,9 @@
       <c r="D14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
         <v>57</v>
@@ -939,7 +949,9 @@
       <c r="D16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
         <v>59</v>

</xml_diff>

<commit_message>
Tuxedo Round 1 results
</commit_message>
<xml_diff>
--- a/2025_results.xlsx
+++ b/2025_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nbr37_newcastle_ac_uk/Documents/MEP and Teaching/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="838" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2D76453-7F4A-4836-8812-0ABEDB806078}"/>
+  <xr:revisionPtr revIDLastSave="846" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{896943A0-0173-4730-A083-1C2F085A4FE9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
   <si>
     <t>Round_1</t>
   </si>
@@ -650,7 +650,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,9 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3"/>
+      <c r="O2" s="3" t="s">
+        <v>45</v>
+      </c>
       <c r="P2" s="3" t="s">
         <v>45</v>
       </c>
@@ -746,7 +748,9 @@
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="3"/>
+      <c r="O4" s="3" t="s">
+        <v>47</v>
+      </c>
       <c r="P4" s="3" t="s">
         <v>47</v>
       </c>
@@ -780,7 +784,9 @@
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="O6" s="3"/>
+      <c r="O6" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="P6" s="3" t="s">
         <v>49</v>
       </c>
@@ -815,7 +821,9 @@
         <v>18</v>
       </c>
       <c r="H8" s="1"/>
-      <c r="O8" s="3"/>
+      <c r="O8" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="P8" s="3" t="s">
         <v>51</v>
       </c>
@@ -849,7 +857,9 @@
       <c r="E10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="O10" s="3"/>
+      <c r="O10" s="3" t="s">
+        <v>53</v>
+      </c>
       <c r="P10" s="3" t="s">
         <v>53</v>
       </c>
@@ -883,7 +893,9 @@
       <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="O12" s="3"/>
+      <c r="O12" s="3" t="s">
+        <v>55</v>
+      </c>
       <c r="P12" s="3" t="s">
         <v>55</v>
       </c>
@@ -918,7 +930,9 @@
       <c r="E14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O14" s="3"/>
+      <c r="O14" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="P14" s="3" t="s">
         <v>57</v>
       </c>
@@ -952,7 +966,9 @@
       <c r="E16" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="3"/>
+      <c r="O16" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="P16" s="3" t="s">
         <v>59</v>
       </c>

</xml_diff>

<commit_message>
Round 2 results and updated the code to work with the ginkgo Rhizo combo
</commit_message>
<xml_diff>
--- a/2025_results.xlsx
+++ b/2025_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://newcastle-my.sharepoint.com/personal/nbr37_newcastle_ac_uk/Documents/MEP and Teaching/MMM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="846" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{896943A0-0173-4730-A083-1C2F085A4FE9}"/>
+  <xr:revisionPtr revIDLastSave="855" documentId="8_{112114C6-7F5F-4BD2-B7B9-FFD9C9F22994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{48346A74-01DD-4984-8EEF-B6FCA48262E5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{3E5A4F85-4087-E24D-A3B4-5C3AA07B2567}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="81">
   <si>
     <t>Round_1</t>
   </si>
@@ -267,9 +267,6 @@
     <t>Fern</t>
   </si>
   <si>
-    <t>GinkoRhizo</t>
-  </si>
-  <si>
     <t>Ceolacanth</t>
   </si>
   <si>
@@ -277,6 +274,9 @@
   </si>
   <si>
     <t>Asain Forest Tortoise</t>
+  </si>
+  <si>
+    <t>GinkgoRhizo</t>
   </si>
 </sst>
 </file>
@@ -650,7 +650,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1018,7 +1018,7 @@
       </c>
       <c r="J19" s="3"/>
       <c r="O19" s="3" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="P19" s="3" t="s">
         <v>61</v>
@@ -1037,8 +1037,12 @@
       <c r="D20" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F20" s="3"/>
-      <c r="N20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="N20" s="3" t="s">
+        <v>80</v>
+      </c>
       <c r="P20" s="3" t="s">
         <v>62</v>
       </c>
@@ -1057,7 +1061,7 @@
         <v>31</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>63</v>
@@ -1093,7 +1097,7 @@
         <v>33</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="P23" s="3" t="s">
         <v>65</v>
@@ -1109,8 +1113,12 @@
       <c r="D24" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F24" s="3"/>
-      <c r="N24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="P24" s="3" t="s">
         <v>66</v>
       </c>
@@ -1129,7 +1137,7 @@
         <v>35</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P25" s="3" t="s">
         <v>67</v>
@@ -1181,8 +1189,12 @@
       <c r="D28" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="3"/>
-      <c r="N28" s="3"/>
+      <c r="F28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N28" s="3" t="s">
+        <v>71</v>
+      </c>
       <c r="P28" s="3" t="s">
         <v>70</v>
       </c>
@@ -1254,8 +1266,12 @@
       <c r="D32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="N32" s="3"/>
+      <c r="F32" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="P32" s="3" t="s">
         <v>74</v>
       </c>

</xml_diff>